<commit_message>
Create proper Office document templates with complete structure for Excel and PowerPoint
</commit_message>
<xml_diff>
--- a/public/templates/blank.xlsx
+++ b/public/templates/blank.xlsx
@@ -7,8 +7,50 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+</file>
+
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+</styleSheet>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetData/>
 </worksheet>
 </file>
</xml_diff>